<commit_message>
maybe finished faro shuffle.
</commit_message>
<xml_diff>
--- a/calc_results.xlsx
+++ b/calc_results.xlsx
@@ -7,13 +7,34 @@
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1 (2)" sheetId="4" r:id="rId1"/>
+    <sheet name="faro" sheetId="4" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>1/2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1/3 - 1/2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1/3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1/3 up down</t>
+    <phoneticPr fontId="1"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -54,8 +75,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -93,9 +115,12 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>1/2-fix</c:v>
+          </c:tx>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet1 (2)'!$A$1:$A$30</c:f>
+              <c:f>faro!$A$2:$A$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -197,9 +222,12 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>1/2-1/3</c:v>
+          </c:tx>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet1 (2)'!$B$1:$B$30</c:f>
+              <c:f>faro!$B$2:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -210,88 +238,302 @@
                   <c:v>1.5560591480255901</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.9459479448872501</c:v>
+                  <c:v>2.8190709892898802</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0042372585122199</c:v>
+                  <c:v>2.9337477147264699</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>3.1726919534566602</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.1460861156381199</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.3621407911402899</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.4076570994091901</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.4222850013982602</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.1864500858913498</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.4870152558011198</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.37100940374647</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.4253943246215401</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.4692780305887601</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.4781466431949402</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.51051177039637</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.4369129033873298</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.3105617178048901</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.39878848680301</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.5004699125521999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.4750373199716602</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.44267219277023</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.4457815159935099</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.49277454518402</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.2477675413873102</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.4268710455431499</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.2870652032096399</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.4122431435540799</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.3841605848139298</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.3945059183417201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>1/3-fix</c:v>
+          </c:tx>
+          <c:yVal>
+            <c:numRef>
+              <c:f>faro!$C$2:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1.09832334990026</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8740628615321699</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4100614480460201</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.98439186933581</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9397453306212999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.15643144916592</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0739317327713702</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.02471159378831</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.2271922318559598</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.3251896197939699</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.0638898749271899</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.21491082034288</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.15143499253031</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.1986180792728098</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.0943189241433302</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.0962550021286201</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.2423117276880302</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.2477675413873102</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.2300303161749602</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.2477675413873102</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.14324803131912</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.10940618319608</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.91025120013121</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.50382897281807</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.0825243124052002</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.5982715335872999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.2503589748378401</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.85287700811362399</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.71918287541957504</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>1/3-up-down</c:v>
+          </c:tx>
+          <c:yVal>
+            <c:numRef>
+              <c:f>faro!$D$2:$D$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>1.09832334990026</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7256267331044199</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8431093060806898</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8335107731195599</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9730453765487899</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.32712569777925</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.4064838541711899</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.2724373012205699</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.2681547327592799</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.39878848680301</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.3136710410281802</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.3798780163526501</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.4515408053764101</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.4515408053764101</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.3251896197939699</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.3640768691255798</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.4022012857099</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>3.3517954576125</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.29593381581582</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.45465012859969</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.4153524667773598</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.3036291831839999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.27702334536546</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.4122431435540799</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.3563815017573999</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3.5709594563379499</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.3563815017573999</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.39878848680301</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3.2612221981383902</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.4503675601384098</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3.2199884583307798</c:v>
-                </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.4222850013982602</c:v>
+                  <c:v>3.4311536140044399</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.44002222661062</c:v>
+                  <c:v>3.3664233596015798</c:v>
                 </c:pt>
                 <c:pt idx="20">
+                  <c:v>3.4488908392167898</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.3784012954310398</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.6222350539897401</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.4635187412058701</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.4827326873398401</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.4604094179825799</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>3.4311536140044399</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>3.3930291974201099</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>3.3841605848139298</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3.37100940374647</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3.3182570851730699</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>3.29593381581582</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3.4604094179825799</c:v>
-                </c:pt>
                 <c:pt idx="27">
-                  <c:v>3.3517954576125</c:v>
+                  <c:v>3.3340582324001402</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3.4503675601384098</c:v>
+                  <c:v>3.4134163887920801</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.4958838684072999</c:v>
+                  <c:v>3.4515408053764101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -306,13 +548,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="139502720"/>
-        <c:axId val="139503296"/>
+        <c:axId val="196542464"/>
+        <c:axId val="134896960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="139502720"/>
+        <c:axId val="196542464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="30"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -338,12 +581,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139503296"/>
+        <c:crossAx val="134896960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="139503296"/>
+        <c:axId val="134896960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -373,11 +616,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139502720"/>
+        <c:crossAx val="196542464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -522,11 +770,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="191195392"/>
-        <c:axId val="191195968"/>
+        <c:axId val="196543616"/>
+        <c:axId val="196544192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="191195392"/>
+        <c:axId val="196543616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -548,18 +796,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191195968"/>
+        <c:crossAx val="196544192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="191195968"/>
+        <c:axId val="196544192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -582,14 +829,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191195392"/>
+        <c:crossAx val="196543616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -610,16 +856,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>83820</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>365760</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -965,252 +1211,452 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B31"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="Q47" sqref="Q47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>0.69300353679601701</v>
       </c>
-      <c r="B1">
+      <c r="B2">
         <v>0.69300353679601701</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="C2">
+        <v>1.09832334990026</v>
+      </c>
+      <c r="D2">
+        <v>1.09832334990026</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>0.54793380569761696</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>1.5560591480255901</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="C3">
+        <v>2.8740628615321699</v>
+      </c>
+      <c r="D3">
+        <v>2.7256267331044199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>0.660471397435901</v>
       </c>
-      <c r="B3">
-        <v>2.9459479448872501</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="B4">
+        <v>2.8190709892898802</v>
+      </c>
+      <c r="C4">
+        <v>2.4100614480460201</v>
+      </c>
+      <c r="D4">
+        <v>2.8431093060806898</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>0.61511123412592905</v>
       </c>
-      <c r="B4">
-        <v>3.0042372585122199</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="B5">
+        <v>2.9337477147264699</v>
+      </c>
+      <c r="C5">
+        <v>2.98439186933581</v>
+      </c>
+      <c r="D5">
+        <v>2.8335107731195599</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>0.64035863593731202</v>
       </c>
-      <c r="B5">
+      <c r="B6">
+        <v>3.1726919534566602</v>
+      </c>
+      <c r="C6">
+        <v>2.9397453306212999</v>
+      </c>
+      <c r="D6">
+        <v>2.9730453765487899</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>0.62839305799521294</v>
+      </c>
+      <c r="B7">
+        <v>3.1460861156381199</v>
+      </c>
+      <c r="C7">
+        <v>3.15643144916592</v>
+      </c>
+      <c r="D7">
+        <v>3.32712569777925</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>0.42709385971193498</v>
+      </c>
+      <c r="B8">
+        <v>3.3621407911402899</v>
+      </c>
+      <c r="C8">
+        <v>3.0739317327713702</v>
+      </c>
+      <c r="D8">
+        <v>3.4064838541711899</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>0.24790180607071099</v>
+      </c>
+      <c r="B9">
+        <v>3.4076570994091901</v>
+      </c>
+      <c r="C9">
+        <v>3.02471159378831</v>
+      </c>
+      <c r="D9">
+        <v>3.2724373012205699</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>0.689551947775073</v>
+      </c>
+      <c r="B10">
+        <v>3.4222850013982602</v>
+      </c>
+      <c r="C10">
+        <v>3.2271922318559598</v>
+      </c>
+      <c r="D10">
+        <v>3.2681547327592799</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>0.52733666618540798</v>
+      </c>
+      <c r="B11">
+        <v>3.1864500858913498</v>
+      </c>
+      <c r="C11">
+        <v>3.3251896197939699</v>
+      </c>
+      <c r="D11">
+        <v>3.39878848680301</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>0.32879120265773998</v>
+      </c>
+      <c r="B12">
+        <v>3.4870152558011198</v>
+      </c>
+      <c r="C12">
+        <v>3.0638898749271899</v>
+      </c>
+      <c r="D12">
+        <v>3.3136710410281802</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>0.68609236734720402</v>
+      </c>
+      <c r="B13">
+        <v>3.37100940374647</v>
+      </c>
+      <c r="C13">
+        <v>3.21491082034288</v>
+      </c>
+      <c r="D13">
+        <v>3.3798780163526501</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>0.58443533321657204</v>
+      </c>
+      <c r="B14">
+        <v>3.4253943246215401</v>
+      </c>
+      <c r="C14">
+        <v>3.15143499253031</v>
+      </c>
+      <c r="D14">
+        <v>3.4515408053764101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>0.65104176150242199</v>
+      </c>
+      <c r="B15">
+        <v>3.4692780305887601</v>
+      </c>
+      <c r="C15">
+        <v>3.1986180792728098</v>
+      </c>
+      <c r="D15">
+        <v>3.4515408053764101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>0.45507904496739399</v>
+      </c>
+      <c r="B16">
+        <v>3.4781466431949402</v>
+      </c>
+      <c r="C16">
+        <v>3.0943189241433302</v>
+      </c>
+      <c r="D16">
+        <v>3.3251896197939699</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>0.67566500186368195</v>
+      </c>
+      <c r="B17">
+        <v>3.51051177039637</v>
+      </c>
+      <c r="C17">
+        <v>3.0962550021286201</v>
+      </c>
+      <c r="D17">
+        <v>3.3640768691255798</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>0.600473870738649</v>
+      </c>
+      <c r="B18">
+        <v>3.4369129033873298</v>
+      </c>
+      <c r="C18">
+        <v>3.2423117276880302</v>
+      </c>
+      <c r="D18">
+        <v>3.4022012857099</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>0.39688253539081603</v>
+      </c>
+      <c r="B19">
+        <v>3.3105617178048901</v>
+      </c>
+      <c r="C19">
+        <v>3.2477675413873102</v>
+      </c>
+      <c r="D19">
         <v>3.3517954576125</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>0.62839305799521294</v>
-      </c>
-      <c r="B6">
-        <v>3.29593381581582</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>0.42709385971193498</v>
-      </c>
-      <c r="B7">
-        <v>3.45465012859969</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>0.24790180607071099</v>
-      </c>
-      <c r="B8">
-        <v>3.4153524667773598</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>0.689551947775073</v>
-      </c>
-      <c r="B9">
-        <v>3.3036291831839999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>0.52733666618540798</v>
-      </c>
-      <c r="B10">
-        <v>3.27702334536546</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>0.32879120265773998</v>
-      </c>
-      <c r="B11">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>0.68146704630140498</v>
+      </c>
+      <c r="B20">
+        <v>3.39878848680301</v>
+      </c>
+      <c r="C20">
+        <v>3.2300303161749602</v>
+      </c>
+      <c r="D20">
+        <v>3.4311536140044399</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>0.505065968010316</v>
+      </c>
+      <c r="B21">
+        <v>3.5004699125521999</v>
+      </c>
+      <c r="C21">
+        <v>3.2477675413873102</v>
+      </c>
+      <c r="D21">
+        <v>3.3664233596015798</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>0.66867221084147499</v>
+      </c>
+      <c r="B22">
+        <v>3.4750373199716602</v>
+      </c>
+      <c r="C22">
+        <v>3.14324803131912</v>
+      </c>
+      <c r="D22">
+        <v>3.4488908392167898</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>0.481020553662315</v>
+      </c>
+      <c r="B23">
+        <v>3.44267219277023</v>
+      </c>
+      <c r="C23">
+        <v>3.10940618319608</v>
+      </c>
+      <c r="D23">
+        <v>3.3784012954310398</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>0.29020984938637501</v>
+      </c>
+      <c r="B24">
+        <v>3.4457815159935099</v>
+      </c>
+      <c r="C24">
+        <v>2.91025120013121</v>
+      </c>
+      <c r="D24">
+        <v>3.6222350539897401</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>0.14804224682624001</v>
+      </c>
+      <c r="B25">
+        <v>3.49277454518402</v>
+      </c>
+      <c r="C25">
+        <v>2.50382897281807</v>
+      </c>
+      <c r="D25">
+        <v>3.4635187412058701</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>0.69185389095749406</v>
+      </c>
+      <c r="B26">
+        <v>3.2477675413873102</v>
+      </c>
+      <c r="C26">
+        <v>2.0825243124052002</v>
+      </c>
+      <c r="D26">
+        <v>3.4827326873398401</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>0.56694258104238604</v>
+      </c>
+      <c r="B27">
+        <v>3.4268710455431499</v>
+      </c>
+      <c r="C27">
+        <v>1.5982715335872999</v>
+      </c>
+      <c r="D27">
+        <v>3.4604094179825799</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>0.364214657301966</v>
+      </c>
+      <c r="B28">
+        <v>3.2870652032096399</v>
+      </c>
+      <c r="C28">
+        <v>1.2503589748378401</v>
+      </c>
+      <c r="D28">
+        <v>3.4311536140044399</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>0.20100301090279199</v>
+      </c>
+      <c r="B29">
         <v>3.4122431435540799</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>0.68609236734720402</v>
-      </c>
-      <c r="B12">
-        <v>3.3563815017573999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>0.58443533321657204</v>
-      </c>
-      <c r="B13">
-        <v>3.5709594563379499</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>0.65104176150242199</v>
-      </c>
-      <c r="B14">
-        <v>3.3563815017573999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>0.45507904496739399</v>
-      </c>
-      <c r="B15">
-        <v>3.39878848680301</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>0.67566500186368195</v>
-      </c>
-      <c r="B16">
-        <v>3.2612221981383902</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>0.600473870738649</v>
-      </c>
-      <c r="B17">
-        <v>3.4503675601384098</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>0.39688253539081603</v>
-      </c>
-      <c r="B18">
-        <v>3.2199884583307798</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>0.68146704630140498</v>
-      </c>
-      <c r="B19">
-        <v>3.4222850013982602</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>0.505065968010316</v>
-      </c>
-      <c r="B20">
-        <v>3.44002222661062</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>0.66867221084147499</v>
-      </c>
-      <c r="B21">
-        <v>3.4311536140044399</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>0.481020553662315</v>
-      </c>
-      <c r="B22">
-        <v>3.3930291974201099</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>0.29020984938637501</v>
-      </c>
-      <c r="B23">
+      <c r="C29">
+        <v>0.85287700811362399</v>
+      </c>
+      <c r="D29">
+        <v>3.3340582324001402</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>8.5915501334663094E-2</v>
+      </c>
+      <c r="B30">
         <v>3.3841605848139298</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>0.14804224682624001</v>
-      </c>
-      <c r="B24">
-        <v>3.37100940374647</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>0.69185389095749406</v>
-      </c>
-      <c r="B25">
-        <v>3.3182570851730699</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>0.56694258104238604</v>
-      </c>
-      <c r="B26">
-        <v>3.29593381581582</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>0.364214657301966</v>
-      </c>
-      <c r="B27">
-        <v>3.4604094179825799</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>0.20100301090279199</v>
-      </c>
-      <c r="B28">
-        <v>3.3517954576125</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>8.5915501334663094E-2</v>
-      </c>
-      <c r="B29">
-        <v>3.4503675601384098</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="C30">
+        <v>0.71918287541957504</v>
+      </c>
+      <c r="D30">
+        <v>3.4134163887920801</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
         <v>0</v>
       </c>
-      <c r="B30">
-        <v>3.4958838684072999</v>
+      <c r="B31">
+        <v>3.3945059183417201</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>3.4515408053764101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>